<commit_message>
3 charts in total
</commit_message>
<xml_diff>
--- a/Dat/RawData_iter_4000.xlsx
+++ b/Dat/RawData_iter_4000.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Python\projekt_korepetycje\Dat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MICHAŁ\Desktop\projekt_korepetycje\Dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125A29DF-9B02-4CCF-9D0A-787BFB16A059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12624" windowHeight="6468"/>
+    <workbookView xWindow="3504" yWindow="384" windowWidth="19128" windowHeight="10896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -60,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +129,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,14 +428,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A984" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M1001"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O958" sqref="O958"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">

</xml_diff>